<commit_message>
OrangeHRM Add Test Scenarios
</commit_message>
<xml_diff>
--- a/manual test/Project1 OrangeHRM/manualtest.xlsx
+++ b/manual test/Project1 OrangeHRM/manualtest.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="68">
   <si>
     <t>FUNTIONAL REQUIREMENT</t>
   </si>
@@ -94,6 +94,144 @@
   </si>
   <si>
     <t>ESS user can add photograph</t>
+  </si>
+  <si>
+    <t>3.1.3</t>
+  </si>
+  <si>
+    <t>ESS user can view Contact Details</t>
+  </si>
+  <si>
+    <t>3.1.4</t>
+  </si>
+  <si>
+    <t>ESS user can add Emergency Contact</t>
+  </si>
+  <si>
+    <t>ESS user can add multiple Emergency Contact</t>
+  </si>
+  <si>
+    <t>ESS user can delete Emergency Contact</t>
+  </si>
+  <si>
+    <t>3.1.5</t>
+  </si>
+  <si>
+    <t>ESS user can add Dependent</t>
+  </si>
+  <si>
+    <t>ESS user can add multiple Dependent</t>
+  </si>
+  <si>
+    <t>ESS user can delete Dependent</t>
+  </si>
+  <si>
+    <t>ESS user can add attachment to Dependent</t>
+  </si>
+  <si>
+    <t>3.1.6</t>
+  </si>
+  <si>
+    <t>ESS user can add Immigration details</t>
+  </si>
+  <si>
+    <t>ESS user can add multiple immigration details</t>
+  </si>
+  <si>
+    <t>ESS user can delete immigration details</t>
+  </si>
+  <si>
+    <t>ESS user can add attachment to immigration record</t>
+  </si>
+  <si>
+    <t>3.1.7</t>
+  </si>
+  <si>
+    <t>ESS user can not change job detail ( view only )</t>
+  </si>
+  <si>
+    <t>3.1.8</t>
+  </si>
+  <si>
+    <t>ESS user restricted to chnage Salary Components</t>
+  </si>
+  <si>
+    <t>3.1.9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ESS user can only see the list of supervisors </t>
+  </si>
+  <si>
+    <t>3.1.10</t>
+  </si>
+  <si>
+    <t>ESS user can add work experience</t>
+  </si>
+  <si>
+    <t>ESS user can add multiple work experience</t>
+  </si>
+  <si>
+    <t>ESS user can delete work experience</t>
+  </si>
+  <si>
+    <t>ESS user can add Education</t>
+  </si>
+  <si>
+    <t>ESS user can add multiple entries of education</t>
+  </si>
+  <si>
+    <t>ESS user can delete education</t>
+  </si>
+  <si>
+    <t>ESS user can add skill</t>
+  </si>
+  <si>
+    <t>ESS user can add multiple skill</t>
+  </si>
+  <si>
+    <t>ESS user can delete skill</t>
+  </si>
+  <si>
+    <t>ESS user can add language</t>
+  </si>
+  <si>
+    <t>ESS user can add multiple language</t>
+  </si>
+  <si>
+    <t>ESS user can delete language</t>
+  </si>
+  <si>
+    <t>ESS user can add license</t>
+  </si>
+  <si>
+    <t>ESS user can add multiple license</t>
+  </si>
+  <si>
+    <t>ESS user can delete license</t>
+  </si>
+  <si>
+    <t>ESS user can upload attachment</t>
+  </si>
+  <si>
+    <t>ESS user can upload multiple attachment</t>
+  </si>
+  <si>
+    <t>ESS user can delete attachment</t>
+  </si>
+  <si>
+    <t>3.1.11</t>
+  </si>
+  <si>
+    <t>ESS user can add membership</t>
+  </si>
+  <si>
+    <t>ESS user can add multiple memberships</t>
+  </si>
+  <si>
+    <t>ESS user can delete memberships</t>
+  </si>
+  <si>
+    <t>ESS user can add attachment under memberships</t>
   </si>
 </sst>
 </file>
@@ -1860,8 +1998,8 @@
   <sheetPr/>
   <dimension ref="A1:C53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="2"/>
@@ -1935,206 +2073,413 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:3">
       <c r="A7" s="2">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
+        <v>22</v>
+      </c>
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" s="2">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
+        <v>22</v>
+      </c>
+      <c r="C8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" s="2">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
+        <v>24</v>
+      </c>
+      <c r="C9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10" s="2">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1">
+        <v>24</v>
+      </c>
+      <c r="C10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11" s="2">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:1">
+      <c r="B11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12" s="2">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:1">
+      <c r="B12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
       <c r="A13" s="2">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:1">
+      <c r="B13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
       <c r="A14" s="2">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:1">
+      <c r="B14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
       <c r="A15" s="2">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:1">
+      <c r="B15" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
       <c r="A16" s="2">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:1">
+      <c r="B16" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
       <c r="A17" s="2">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:1">
+      <c r="B17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
       <c r="A18" s="2">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:1">
+      <c r="B18" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
       <c r="A19" s="2">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:1">
+      <c r="B19" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
       <c r="A20" s="2">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:1">
+      <c r="B20" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
       <c r="A21" s="2">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:1">
+      <c r="B21" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
       <c r="A22" s="2">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:1">
+      <c r="B22" t="s">
+        <v>42</v>
+      </c>
+      <c r="C22" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
       <c r="A23" s="2">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:1">
+      <c r="B23" t="s">
+        <v>44</v>
+      </c>
+      <c r="C23" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
       <c r="A24" s="2">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:1">
+      <c r="B24" t="s">
+        <v>44</v>
+      </c>
+      <c r="C24" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
       <c r="A25" s="2">
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="1:1">
+      <c r="B25" t="s">
+        <v>44</v>
+      </c>
+      <c r="C25" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
       <c r="A26" s="2">
         <v>25</v>
       </c>
-    </row>
-    <row r="27" spans="1:1">
+      <c r="B26" t="s">
+        <v>44</v>
+      </c>
+      <c r="C26" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
       <c r="A27" s="2">
         <v>26</v>
       </c>
-    </row>
-    <row r="28" spans="1:1">
+      <c r="B27" t="s">
+        <v>44</v>
+      </c>
+      <c r="C27" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
       <c r="A28" s="2">
         <v>27</v>
       </c>
-    </row>
-    <row r="29" spans="1:1">
+      <c r="B28" t="s">
+        <v>44</v>
+      </c>
+      <c r="C28" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
       <c r="A29" s="2">
         <v>28</v>
       </c>
-    </row>
-    <row r="30" spans="1:1">
+      <c r="B29" t="s">
+        <v>44</v>
+      </c>
+      <c r="C29" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
       <c r="A30" s="2">
         <v>29</v>
       </c>
-    </row>
-    <row r="31" spans="1:1">
+      <c r="B30" t="s">
+        <v>44</v>
+      </c>
+      <c r="C30" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
       <c r="A31" s="2">
         <v>30</v>
       </c>
-    </row>
-    <row r="32" spans="1:1">
+      <c r="B31" t="s">
+        <v>44</v>
+      </c>
+      <c r="C31" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
       <c r="A32" s="2">
         <v>31</v>
       </c>
-    </row>
-    <row r="33" spans="1:1">
+      <c r="B32" t="s">
+        <v>44</v>
+      </c>
+      <c r="C32" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
       <c r="A33" s="2">
         <v>32</v>
       </c>
-    </row>
-    <row r="34" spans="1:1">
+      <c r="B33" t="s">
+        <v>44</v>
+      </c>
+      <c r="C33" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
       <c r="A34" s="2">
         <v>33</v>
       </c>
-    </row>
-    <row r="35" spans="1:1">
+      <c r="B34" t="s">
+        <v>44</v>
+      </c>
+      <c r="C34" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
       <c r="A35" s="2">
         <v>34</v>
       </c>
-    </row>
-    <row r="36" spans="1:1">
+      <c r="B35" t="s">
+        <v>44</v>
+      </c>
+      <c r="C35" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
       <c r="A36" s="2">
         <v>35</v>
       </c>
-    </row>
-    <row r="37" spans="1:1">
+      <c r="B36" t="s">
+        <v>44</v>
+      </c>
+      <c r="C36" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
       <c r="A37" s="2">
         <v>36</v>
       </c>
-    </row>
-    <row r="38" spans="1:1">
+      <c r="B37" t="s">
+        <v>44</v>
+      </c>
+      <c r="C37" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
       <c r="A38" s="2">
         <v>37</v>
       </c>
-    </row>
-    <row r="39" spans="1:1">
+      <c r="B38" t="s">
+        <v>44</v>
+      </c>
+      <c r="C38" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
       <c r="A39" s="2">
         <v>38</v>
       </c>
-    </row>
-    <row r="40" spans="1:1">
+      <c r="B39" t="s">
+        <v>44</v>
+      </c>
+      <c r="C39" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
       <c r="A40" s="2">
         <v>39</v>
       </c>
-    </row>
-    <row r="41" spans="1:1">
+      <c r="B40" t="s">
+        <v>44</v>
+      </c>
+      <c r="C40" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
       <c r="A41" s="2">
         <v>40</v>
       </c>
-    </row>
-    <row r="42" spans="1:1">
+      <c r="B41" t="s">
+        <v>63</v>
+      </c>
+      <c r="C41" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
       <c r="A42" s="2">
         <v>41</v>
       </c>
-    </row>
-    <row r="43" spans="1:1">
+      <c r="C42" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
       <c r="A43" s="2">
         <v>42</v>
       </c>
-    </row>
-    <row r="44" spans="1:1">
+      <c r="C43" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
       <c r="A44" s="2">
         <v>43</v>
+      </c>
+      <c r="C44" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="45" spans="1:1">

</xml_diff>